<commit_message>
Update Personal Budget Spreadsheet.xlsx
</commit_message>
<xml_diff>
--- a/Personal Budget Spreadsheet.xlsx
+++ b/Personal Budget Spreadsheet.xlsx
@@ -501,7 +501,7 @@
     <numFmt numFmtId="168" formatCode="d/mmm/yy"/>
     <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="170" formatCode="mmmm"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -1388,59 +1388,11 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="170" fontId="23" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1460,6 +1412,54 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="170" fontId="23" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1683,9 +1683,73 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="d/mmmm/yy"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="d/mmm/yy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="2" tint="-0.499984740745262"/>
       </font>
-      <numFmt numFmtId="171" formatCode="\➜\ d/mmm/yy"/>
+      <numFmt numFmtId="172" formatCode="\➜\ d/mmm/yy"/>
     </dxf>
     <dxf>
       <font>
@@ -1693,12 +1757,174 @@
         <i val="0"/>
         <color rgb="FF92D050"/>
       </font>
-      <numFmt numFmtId="172" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+      <numFmt numFmtId="173" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1974,232 +2200,6 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="d/mmmm/yy"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="d/mmm/yy"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -9888,7 +9888,7 @@
                 <a:cs typeface="Calibri"/>
               </a:rPr>
               <a:pPr/>
-              <a:t>07-Sep-24</a:t>
+              <a:t>10-Sep-24</a:t>
             </a:fld>
             <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
           </a:p>
@@ -10120,7 +10120,7 @@
                 <a:cs typeface="Calibri"/>
               </a:rPr>
               <a:pPr/>
-              <a:t>(247 days ago)</a:t>
+              <a:t>(250 days ago)</a:t>
             </a:fld>
             <a:endParaRPr lang="en-CA" sz="1000" b="1"/>
           </a:p>
@@ -12001,6 +12001,7 @@
                 <a:latin typeface="Calibri"/>
                 <a:cs typeface="Calibri"/>
               </a:rPr>
+              <a:pPr/>
               <a:t>-880 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-CA" sz="900" b="1"/>
@@ -12050,6 +12051,7 @@
                 <a:latin typeface="Calibri"/>
                 <a:cs typeface="Calibri"/>
               </a:rPr>
+              <a:pPr/>
               <a:t>allocated not covered by income</a:t>
             </a:fld>
             <a:endParaRPr lang="en-CA" sz="900" b="1"/>
@@ -12227,6 +12229,7 @@
                 <a:latin typeface="Calibri"/>
                 <a:cs typeface="Calibri"/>
               </a:rPr>
+              <a:pPr/>
               <a:t>22.1%</a:t>
             </a:fld>
             <a:endParaRPr lang="en-CA" sz="1000" b="1">
@@ -12373,57 +12376,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Income" displayName="Income" ref="C9:C12" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Income" displayName="Income" ref="C9:C12" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="C9:C12">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Income" dataDxfId="78"/>
+    <tableColumn id="1" name="Income" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Income Table Sty" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Expenses" displayName="Expenses" ref="C22:C30" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Expenses" displayName="Expenses" ref="C22:C30" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="C22:C30">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Expenses" dataDxfId="75"/>
+    <tableColumn id="1" name="Expenses" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="Expenses Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Savings" displayName="Savings" ref="C40:C45" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Savings" displayName="Savings" ref="C40:C45" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="C40:C45">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Savings" dataDxfId="72"/>
+    <tableColumn id="1" name="Savings" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="Savings Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tracking" displayName="Tracking" ref="C11:I66" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tracking" displayName="Tracking" ref="C11:I66" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="C11:I66"/>
   <sortState ref="C12:I66">
     <sortCondition ref="C11:C66"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Date" dataDxfId="69"/>
-    <tableColumn id="2" name="Type" dataDxfId="68"/>
-    <tableColumn id="3" name="Category" dataDxfId="67"/>
-    <tableColumn id="4" name="Amount" dataDxfId="66" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="Details" dataDxfId="65"/>
-    <tableColumn id="6" name="Balance" dataDxfId="64" dataCellStyle="Comma">
+    <tableColumn id="1" name="Date" dataDxfId="31"/>
+    <tableColumn id="2" name="Type" dataDxfId="30"/>
+    <tableColumn id="3" name="Category" dataDxfId="29"/>
+    <tableColumn id="4" name="Amount" dataDxfId="28" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="Details" dataDxfId="27"/>
+    <tableColumn id="6" name="Balance" dataDxfId="26" dataCellStyle="Comma">
       <calculatedColumnFormula>SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]), (Tracking[Type]&lt;&gt;"Income")*(-1)+(Tracking[Type]="Income"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Effective Date" dataDxfId="63">
+    <tableColumn id="7" name="Effective Date" dataDxfId="25">
       <calculatedColumnFormula>IF(AND(Tracking[[#This Row],[Type]]="Income", shift_late_income_status="Active", DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day), DATE(YEAR(Tracking[[#This Row],[Date]]), MONTH(Tracking[[#This Row],[Date]])+1,1), Tracking[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12710,22 +12713,22 @@
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="109" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" s="109" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="31"/>
@@ -12758,14 +12761,14 @@
       <c r="H8" s="35"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="127"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="31"/>
@@ -12802,7 +12805,7 @@
         <v>90</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="111" t="s">
+      <c r="G15" s="125" t="s">
         <v>116</v>
       </c>
       <c r="H15" s="32"/>
@@ -12812,7 +12815,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="111"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
@@ -12824,7 +12827,7 @@
         <v>25</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="111"/>
+      <c r="G17" s="125"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
@@ -12837,7 +12840,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="31"/>
-      <c r="D19" s="126" t="s">
+      <c r="D19" s="110" t="s">
         <v>113</v>
       </c>
       <c r="E19" s="1"/>
@@ -12862,7 +12865,7 @@
         <v>115</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="111" t="s">
+      <c r="G21" s="125" t="s">
         <v>117</v>
       </c>
       <c r="H21" s="32"/>
@@ -12872,7 +12875,7 @@
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="111"/>
+      <c r="G22" s="125"/>
       <c r="H22" s="32"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
@@ -12880,7 +12883,7 @@
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="111"/>
+      <c r="G23" s="125"/>
       <c r="H23" s="32"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
@@ -12900,7 +12903,7 @@
     <mergeCell ref="G15:G17"/>
   </mergeCells>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="62" priority="1">
+    <cfRule type="expression" dxfId="80" priority="1">
       <formula>shift_late_income_status = "Inactive"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12946,106 +12949,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
     </row>
     <row r="2" spans="1:73" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
+      <c r="A2" s="126"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
     </row>
     <row r="3" spans="1:73" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="109"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
+      <c r="A3" s="126"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="110">
+      <c r="E5" s="127">
         <f>starting_year</f>
         <v>2022</v>
       </c>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="110"/>
-      <c r="N5" s="110"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="S5" s="110">
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127"/>
+      <c r="S5" s="127">
         <f>starting_year+1</f>
         <v>2023</v>
       </c>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
-      <c r="Y5" s="110"/>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="110"/>
-      <c r="AB5" s="110"/>
-      <c r="AC5" s="110"/>
-      <c r="AD5" s="110"/>
-      <c r="AE5" s="110"/>
-      <c r="AG5" s="110">
+      <c r="T5" s="127"/>
+      <c r="U5" s="127"/>
+      <c r="V5" s="127"/>
+      <c r="W5" s="127"/>
+      <c r="X5" s="127"/>
+      <c r="Y5" s="127"/>
+      <c r="Z5" s="127"/>
+      <c r="AA5" s="127"/>
+      <c r="AB5" s="127"/>
+      <c r="AC5" s="127"/>
+      <c r="AD5" s="127"/>
+      <c r="AE5" s="127"/>
+      <c r="AG5" s="127">
         <f>starting_year+2</f>
         <v>2024</v>
       </c>
-      <c r="AH5" s="110"/>
-      <c r="AI5" s="110"/>
-      <c r="AJ5" s="110"/>
-      <c r="AK5" s="110"/>
-      <c r="AL5" s="110"/>
-      <c r="AM5" s="110"/>
-      <c r="AN5" s="110"/>
-      <c r="AO5" s="110"/>
-      <c r="AP5" s="110"/>
-      <c r="AQ5" s="110"/>
-      <c r="AR5" s="110"/>
-      <c r="AS5" s="110"/>
-      <c r="AU5" s="110">
+      <c r="AH5" s="127"/>
+      <c r="AI5" s="127"/>
+      <c r="AJ5" s="127"/>
+      <c r="AK5" s="127"/>
+      <c r="AL5" s="127"/>
+      <c r="AM5" s="127"/>
+      <c r="AN5" s="127"/>
+      <c r="AO5" s="127"/>
+      <c r="AP5" s="127"/>
+      <c r="AQ5" s="127"/>
+      <c r="AR5" s="127"/>
+      <c r="AS5" s="127"/>
+      <c r="AU5" s="127">
         <f>starting_year+3</f>
         <v>2025</v>
       </c>
-      <c r="AV5" s="110"/>
-      <c r="AW5" s="110"/>
-      <c r="AX5" s="110"/>
-      <c r="AY5" s="110"/>
-      <c r="AZ5" s="110"/>
-      <c r="BA5" s="110"/>
-      <c r="BB5" s="110"/>
-      <c r="BC5" s="110"/>
-      <c r="BD5" s="110"/>
-      <c r="BE5" s="110"/>
-      <c r="BF5" s="110"/>
-      <c r="BG5" s="110"/>
-      <c r="BI5" s="110">
+      <c r="AV5" s="127"/>
+      <c r="AW5" s="127"/>
+      <c r="AX5" s="127"/>
+      <c r="AY5" s="127"/>
+      <c r="AZ5" s="127"/>
+      <c r="BA5" s="127"/>
+      <c r="BB5" s="127"/>
+      <c r="BC5" s="127"/>
+      <c r="BD5" s="127"/>
+      <c r="BE5" s="127"/>
+      <c r="BF5" s="127"/>
+      <c r="BG5" s="127"/>
+      <c r="BI5" s="127">
         <f>starting_year+4</f>
         <v>2026</v>
       </c>
-      <c r="BJ5" s="110"/>
-      <c r="BK5" s="110"/>
-      <c r="BL5" s="110"/>
-      <c r="BM5" s="110"/>
-      <c r="BN5" s="110"/>
-      <c r="BO5" s="110"/>
-      <c r="BP5" s="110"/>
-      <c r="BQ5" s="110"/>
-      <c r="BR5" s="110"/>
-      <c r="BS5" s="110"/>
-      <c r="BT5" s="110"/>
-      <c r="BU5" s="110"/>
+      <c r="BJ5" s="127"/>
+      <c r="BK5" s="127"/>
+      <c r="BL5" s="127"/>
+      <c r="BM5" s="127"/>
+      <c r="BN5" s="127"/>
+      <c r="BO5" s="127"/>
+      <c r="BP5" s="127"/>
+      <c r="BQ5" s="127"/>
+      <c r="BR5" s="127"/>
+      <c r="BS5" s="127"/>
+      <c r="BT5" s="127"/>
+      <c r="BU5" s="127"/>
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E6" s="22" t="str">
@@ -18381,152 +18384,152 @@
     <mergeCell ref="AU5:BG5"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C19 Q10:Q20 E10:P19">
-    <cfRule type="expression" dxfId="61" priority="34">
+    <cfRule type="expression" dxfId="79" priority="34">
       <formula>ROW(C10) &lt;= income_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C30 Q23:Q38 E23:P37">
-    <cfRule type="expression" dxfId="60" priority="33">
+    <cfRule type="expression" dxfId="78" priority="33">
       <formula>ROW(C23) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41:Q51 C41:C45 E41:P50">
-    <cfRule type="expression" dxfId="59" priority="32">
+    <cfRule type="expression" dxfId="77" priority="32">
       <formula>ROW(C41) &lt;= savings_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="58" priority="31">
+    <cfRule type="expression" dxfId="76" priority="31">
       <formula>ROW(C47) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="57" priority="30">
+    <cfRule type="expression" dxfId="75" priority="30">
       <formula>ROW(C48) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="56" priority="29">
+    <cfRule type="expression" dxfId="74" priority="29">
       <formula>ROW(C49) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="55" priority="28">
+    <cfRule type="expression" dxfId="73" priority="28">
       <formula>ROW(C50) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:Q7">
-    <cfRule type="expression" dxfId="54" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="25" stopIfTrue="1">
       <formula>AND(E$20 = 0,E$38 = 0,E$51 = 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="26" stopIfTrue="1">
       <formula>E$7 = 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="27">
+    <cfRule type="expression" dxfId="70" priority="27">
       <formula>E$7 &lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE10:AE20 S10:AD19">
-    <cfRule type="expression" dxfId="51" priority="24">
+    <cfRule type="expression" dxfId="69" priority="24">
       <formula>ROW(S10) &lt;= income_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE23:AE38 S23:AD37">
-    <cfRule type="expression" dxfId="50" priority="23">
+    <cfRule type="expression" dxfId="68" priority="23">
       <formula>ROW(S23) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE41:AE51 S41:AD50">
-    <cfRule type="expression" dxfId="49" priority="22">
+    <cfRule type="expression" dxfId="67" priority="22">
       <formula>ROW(S41) &lt;= savings_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:AE7">
-    <cfRule type="expression" dxfId="48" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="19" stopIfTrue="1">
       <formula>AND(S$20 = 0,S$38 = 0,S$51 = 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="20" stopIfTrue="1">
       <formula>S$7 = 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="21">
+    <cfRule type="expression" dxfId="64" priority="21">
       <formula>S$7 &lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS10:AS20 AG10:AR19">
-    <cfRule type="expression" dxfId="45" priority="18">
+    <cfRule type="expression" dxfId="63" priority="18">
       <formula>ROW(AG10) &lt;= income_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS23:AS38 AG23:AR37">
-    <cfRule type="expression" dxfId="44" priority="17">
+    <cfRule type="expression" dxfId="62" priority="17">
       <formula>ROW(AG23) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS41:AS51 AG41:AR50">
-    <cfRule type="expression" dxfId="43" priority="16">
+    <cfRule type="expression" dxfId="61" priority="16">
       <formula>ROW(AG41) &lt;= savings_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG6:AS7">
-    <cfRule type="expression" dxfId="42" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="13" stopIfTrue="1">
       <formula>AND(AG$20 = 0,AG$38 = 0,AG$51 = 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="14" stopIfTrue="1">
       <formula>AG$7 = 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="15">
+    <cfRule type="expression" dxfId="58" priority="15">
       <formula>AG$7 &lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG10:BG20 AU10:BF19">
-    <cfRule type="expression" dxfId="39" priority="12">
+    <cfRule type="expression" dxfId="57" priority="12">
       <formula>ROW(AU10) &lt;= income_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG23:BG38 AU23:BF37">
-    <cfRule type="expression" dxfId="38" priority="11">
+    <cfRule type="expression" dxfId="56" priority="11">
       <formula>ROW(AU23) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG41:BG51 AU41:BF50">
-    <cfRule type="expression" dxfId="37" priority="10">
+    <cfRule type="expression" dxfId="55" priority="10">
       <formula>ROW(AU41) &lt;= savings_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU6:BG7">
-    <cfRule type="expression" dxfId="36" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="7" stopIfTrue="1">
       <formula>AND(AU$20 = 0,AU$38 = 0,AU$51 = 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="8" stopIfTrue="1">
       <formula>AU$7 = 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="9">
+    <cfRule type="expression" dxfId="52" priority="9">
       <formula>AU$7 &lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU10:BU20 BI10:BT19">
-    <cfRule type="expression" dxfId="33" priority="6">
+    <cfRule type="expression" dxfId="51" priority="6">
       <formula>ROW(BI10) &lt;= income_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU23:BU38 BI23:BT37">
-    <cfRule type="expression" dxfId="32" priority="5">
+    <cfRule type="expression" dxfId="50" priority="5">
       <formula>ROW(BI23) &lt;= expense_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU41:BU51 BI41:BT50">
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="49" priority="4">
       <formula>ROW(BI41) &lt;= savings_max_row</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI6:BU7">
-    <cfRule type="expression" dxfId="30" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="1" stopIfTrue="1">
       <formula>AND(BI$20 = 0,BI$38 = 0,BI$51 = 0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="2" stopIfTrue="1">
       <formula>BI$7 = 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="46" priority="3">
       <formula>BI$7 &lt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18561,13 +18564,13 @@
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:9" s="126" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" s="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" s="126" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="25" t="s">
         <v>32</v>
@@ -19857,17 +19860,17 @@
     <mergeCell ref="A1:XFD3"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:E66">
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="36" priority="8">
       <formula>ISNA(MATCH(E12, INDIRECT(D12), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F66">
-    <cfRule type="expression" dxfId="26" priority="5">
+    <cfRule type="expression" dxfId="35" priority="5">
       <formula>D12="Income"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I66">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="34" priority="1">
       <formula>AND(D12="Income", shift_late_income_status="Active", DAY(C12)&gt;=shift_late_income_starting_day)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19941,35 +19944,35 @@
     <col min="43" max="43" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="109" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:44" s="126" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:44" s="109" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:44" s="109" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:44" s="126" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:44" s="126" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AQ5" s="112" t="s">
+      <c r="AQ5" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="AR5" s="113"/>
+      <c r="AR5" s="133"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN6" s="114" t="s">
+      <c r="AN6" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="AO6" s="114"/>
-      <c r="AP6" s="114"/>
-      <c r="AQ6" s="118">
+      <c r="AO6" s="128"/>
+      <c r="AP6" s="128"/>
+      <c r="AQ6" s="134">
         <v>2022</v>
       </c>
-      <c r="AR6" s="118"/>
+      <c r="AR6" s="134"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AQ8" s="112" t="s">
+      <c r="AQ8" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="AR8" s="113"/>
+      <c r="AR8" s="133"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="K9" t="e">
@@ -19985,15 +19988,15 @@
   )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AN9" s="114" t="s">
+      <c r="AN9" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="AO9" s="114"/>
-      <c r="AP9" s="114"/>
-      <c r="AQ9" s="115" t="s">
+      <c r="AO9" s="128"/>
+      <c r="AP9" s="128"/>
+      <c r="AQ9" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="AR9" s="115"/>
+      <c r="AR9" s="129"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C11" s="91"/>
@@ -20018,31 +20021,31 @@
       <c r="V11" s="91"/>
       <c r="W11" s="91"/>
       <c r="X11" s="91"/>
-      <c r="Y11" s="116" t="str">
+      <c r="Y11" s="130" t="str">
         <f>"Breakdown - " &amp; IF(selected_period="Total Year", selected_year &amp; " (Total Year)", selected_period_display &amp; " " &amp; selected_year)</f>
         <v>Breakdown - 2022 (Total Year)</v>
       </c>
-      <c r="Z11" s="117"/>
-      <c r="AA11" s="117"/>
-      <c r="AB11" s="117"/>
-      <c r="AC11" s="117"/>
-      <c r="AD11" s="117"/>
-      <c r="AF11" s="117" t="str">
+      <c r="Z11" s="131"/>
+      <c r="AA11" s="131"/>
+      <c r="AB11" s="131"/>
+      <c r="AC11" s="131"/>
+      <c r="AD11" s="131"/>
+      <c r="AF11" s="131" t="str">
         <f>"Summary - " &amp; IF(selected_period="Total Year", selected_year &amp; " (Total Year)", selected_period_display &amp; " " &amp; selected_year)</f>
         <v>Summary - 2022 (Total Year)</v>
       </c>
-      <c r="AG11" s="117"/>
-      <c r="AH11" s="117"/>
-      <c r="AI11" s="117"/>
-      <c r="AJ11" s="117"/>
-      <c r="AK11" s="117"/>
-      <c r="AL11" s="117"/>
-      <c r="AM11" s="117"/>
-      <c r="AN11" s="117"/>
-      <c r="AO11" s="117"/>
-      <c r="AP11" s="117"/>
-      <c r="AQ11" s="117"/>
-      <c r="AR11" s="117"/>
+      <c r="AG11" s="131"/>
+      <c r="AH11" s="131"/>
+      <c r="AI11" s="131"/>
+      <c r="AJ11" s="131"/>
+      <c r="AK11" s="131"/>
+      <c r="AL11" s="131"/>
+      <c r="AM11" s="131"/>
+      <c r="AN11" s="131"/>
+      <c r="AO11" s="131"/>
+      <c r="AP11" s="131"/>
+      <c r="AQ11" s="131"/>
+      <c r="AR11" s="131"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
@@ -23758,8 +23761,8 @@
       <c r="AQ35" s="1"/>
       <c r="AR35" s="74"/>
     </row>
-    <row r="36" spans="3:44" s="137" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="129">
+    <row r="36" spans="3:44" s="121" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="113">
         <f>IF(C35=-1,-1,
    IF(C35&lt;income_max_row,C35+1,
       IF(C35=income_max_row, income_total_row,
@@ -23774,35 +23777,35 @@
 )))))))))))</f>
         <v>51</v>
       </c>
-      <c r="D36" s="130">
+      <c r="D36" s="114">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E36" s="129">
+      <c r="E36" s="113">
         <f>1*OR(row_id = income_header_row, row_id = expense_header_row, row_id = savings_header_row)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="131">
+      <c r="F36" s="115">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36" s="140">
+      <c r="G36" s="124">
         <f>1*OR(row_id=income_total_row,row_id=expenses_total_row,row_id=savings_total_row)</f>
         <v>1</v>
       </c>
-      <c r="H36" s="131">
+      <c r="H36" s="115">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I36" s="129" t="str">
+      <c r="I36" s="113" t="str">
         <f>IFERROR(INDEX('Budget Planning'!C:C, header_row_id), "")</f>
         <v>Savings</v>
       </c>
-      <c r="J36" s="131" t="str">
+      <c r="J36" s="115" t="str">
         <f>IFERROR(INDEX('Budget Planning'!C:C, row_id), "")</f>
         <v>Total</v>
       </c>
-      <c r="K36" s="132">
+      <c r="K36" s="116">
         <f xml:space="preserve"> IF(OR(is_header,is_empty),"",
       IF(is_total,
           IF(selected_period="Total Year",
@@ -23815,102 +23818,102 @@
   )</f>
         <v>2800</v>
       </c>
-      <c r="L36" s="132">
+      <c r="L36" s="116">
         <f ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$BU,row_id,
    MATCH(IF(selected_period = "Total Year", selected_year, DATE(selected_year, selected_period, 1)),'Budget Planning'!$E$9:$BU$9, 0)))</f>
         <v>21900</v>
       </c>
-      <c r="M36" s="129" t="str">
+      <c r="M36" s="113" t="str">
         <f>IF(is_cat,
 IF(header_row_id=income_header_row,MATCH(income_min_row,$C:$C,0),
 IF(header_row_id=expense_header_row,MATCH(expense_min_row,$C:$C,0),
 IF(header_row_id=savings_header_row,MATCH(savings_min_row,$C:$C,0),""))), "")</f>
         <v/>
       </c>
-      <c r="N36" s="130" t="str">
+      <c r="N36" s="114" t="str">
         <f>IF(is_cat,
 IF(header_row_id=income_header_row,MATCH(income_max_row,$C:$C,0),
 IF(header_row_id=expense_header_row,MATCH(expense_max_row,$C:$C,0),
 IF(header_row_id=savings_header_row,MATCH(savings_max_row,$C:$C,0),""))), "")</f>
         <v/>
       </c>
-      <c r="O36" s="129" t="str">
+      <c r="O36" s="113" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P36" s="131" t="str">
+      <c r="P36" s="115" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="Q36" s="131" t="str">
+      <c r="Q36" s="115" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="R36" s="130" t="str">
+      <c r="R36" s="114" t="str">
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="S36" s="129" t="str">
+      <c r="S36" s="113" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="T36" s="131" t="str">
+      <c r="T36" s="115" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="U36" s="131" t="str">
+      <c r="U36" s="115" t="str">
         <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
-      <c r="V36" s="131" t="str">
+      <c r="V36" s="115" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="W36" s="130" t="str">
+      <c r="W36" s="114" t="str">
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="X36" s="133">
+      <c r="X36" s="117">
         <f t="shared" si="12"/>
         <v>51</v>
       </c>
-      <c r="Y36" s="134" t="str">
+      <c r="Y36" s="118" t="str">
         <f ca="1">IF(is_empty, "", INDEX($J:$J, MATCH(row_id, $X:$X, 0)))</f>
         <v>Total</v>
       </c>
-      <c r="Z36" s="135">
+      <c r="Z36" s="119">
         <f t="shared" ca="1" si="14"/>
         <v>2800</v>
       </c>
-      <c r="AA36" s="135">
+      <c r="AA36" s="119">
         <f t="shared" ca="1" si="15"/>
         <v>21900</v>
       </c>
-      <c r="AB36" s="136">
+      <c r="AB36" s="120">
         <f t="shared" ca="1" si="16"/>
         <v>0.12785388127853881</v>
       </c>
-      <c r="AC36" s="135">
+      <c r="AC36" s="119">
         <f t="shared" ca="1" si="17"/>
         <v>19100</v>
       </c>
-      <c r="AD36" s="135">
+      <c r="AD36" s="119">
         <f t="shared" ca="1" si="18"/>
         <v>0</v>
       </c>
-      <c r="AF36" s="138"/>
-      <c r="AG36" s="131"/>
-      <c r="AH36" s="131"/>
-      <c r="AI36" s="131"/>
-      <c r="AJ36" s="131"/>
-      <c r="AK36" s="139"/>
-      <c r="AM36" s="138"/>
-      <c r="AN36" s="131"/>
-      <c r="AO36" s="131"/>
-      <c r="AP36" s="131"/>
-      <c r="AQ36" s="131"/>
-      <c r="AR36" s="139"/>
+      <c r="AF36" s="122"/>
+      <c r="AG36" s="115"/>
+      <c r="AH36" s="115"/>
+      <c r="AI36" s="115"/>
+      <c r="AJ36" s="115"/>
+      <c r="AK36" s="123"/>
+      <c r="AM36" s="122"/>
+      <c r="AN36" s="115"/>
+      <c r="AO36" s="115"/>
+      <c r="AP36" s="115"/>
+      <c r="AQ36" s="115"/>
+      <c r="AR36" s="123"/>
     </row>
     <row r="37" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C37" s="53">
@@ -23956,7 +23959,7 @@
         <f>IFERROR(INDEX('Budget Planning'!C:C, row_id), "")</f>
         <v/>
       </c>
-      <c r="K37" s="128" t="str">
+      <c r="K37" s="112" t="str">
         <f xml:space="preserve"> IF(OR(is_header,is_empty),"",
       IF(is_total,
           IF(selected_period="Total Year",
@@ -26481,15 +26484,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AN6:AP6"/>
     <mergeCell ref="A1:XFD3"/>
     <mergeCell ref="AQ8:AR8"/>
     <mergeCell ref="AN9:AP9"/>
     <mergeCell ref="AQ9:AR9"/>
     <mergeCell ref="Y11:AD11"/>
     <mergeCell ref="AF11:AR11"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AN6:AP6"/>
   </mergeCells>
   <conditionalFormatting sqref="Y13:AD54">
     <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
@@ -26790,38 +26793,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
       <c r="J1" s="104"/>
       <c r="K1" s="104"/>
       <c r="L1" s="104"/>
     </row>
     <row r="2" spans="2:12" s="38" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
       <c r="J2" s="104"/>
       <c r="K2" s="104"/>
       <c r="L2" s="104"/>
     </row>
     <row r="3" spans="2:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
       <c r="J3" s="104"/>
       <c r="K3" s="104"/>
       <c r="L3" s="104"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="123" t="s">
+      <c r="C6" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D8" s="39" t="s">
@@ -26829,7 +26832,7 @@
       </c>
       <c r="E8" s="40">
         <f ca="1">TODAY()</f>
-        <v>45542</v>
+        <v>45545</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -26847,7 +26850,7 @@
       </c>
       <c r="E10" s="20" t="str">
         <f ca="1">IF(E9=0, "", "(" &amp; _xlfn.DAYS(current_date,E9)&amp; " days ago)")</f>
-        <v>(247 days ago)</v>
+        <v>(250 days ago)</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -26887,12 +26890,12 @@
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D19" s="39" t="s">
@@ -26957,7 +26960,7 @@
       <c r="D25" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="E25" s="125">
+      <c r="E25" s="109">
         <f ca="1">F41-(J41+N41)</f>
         <v>-880</v>
       </c>
@@ -26975,7 +26978,7 @@
       <c r="D27" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="127">
+      <c r="E27" s="111">
         <f ca="1">IFERROR(IF(savings_rate_calculation_type = "% Allocated to Savings", N41 / F41, (F41-J41) / F41), "-")</f>
         <v>0.22068965517241379</v>
       </c>
@@ -27338,16 +27341,16 @@
       </c>
     </row>
     <row r="53" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="M53" s="110" t="s">
+      <c r="M53" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="N53" s="110"/>
-      <c r="O53" s="110"/>
-      <c r="P53" s="122" t="s">
+      <c r="N53" s="127"/>
+      <c r="O53" s="127"/>
+      <c r="P53" s="140" t="s">
         <v>101</v>
       </c>
-      <c r="Q53" s="122"/>
-      <c r="R53" s="122"/>
+      <c r="Q53" s="140"/>
+      <c r="R53" s="140"/>
     </row>
     <row r="54" spans="4:18" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="80" t="s">
@@ -27397,7 +27400,7 @@
       </c>
     </row>
     <row r="55" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D55" s="119">
+      <c r="D55" s="135">
         <f>DATE(selected_year, 1, 1)</f>
         <v>44562</v>
       </c>
@@ -27458,7 +27461,7 @@
       </c>
     </row>
     <row r="56" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D56" s="120"/>
+      <c r="D56" s="136"/>
       <c r="E56" s="99" t="s">
         <v>13</v>
       </c>
@@ -27516,7 +27519,7 @@
       </c>
     </row>
     <row r="57" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D57" s="120"/>
+      <c r="D57" s="136"/>
       <c r="E57" s="99" t="s">
         <v>18</v>
       </c>
@@ -27574,7 +27577,7 @@
       </c>
     </row>
     <row r="58" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D58" s="121"/>
+      <c r="D58" s="137"/>
       <c r="E58" s="100"/>
       <c r="F58" s="100"/>
       <c r="G58" s="100"/>
@@ -27591,7 +27594,7 @@
       <c r="R58" s="100"/>
     </row>
     <row r="59" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D59" s="119">
+      <c r="D59" s="135">
         <f>DATE(selected_year, 2, 1)</f>
         <v>44593</v>
       </c>
@@ -27652,7 +27655,7 @@
       </c>
     </row>
     <row r="60" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D60" s="120"/>
+      <c r="D60" s="136"/>
       <c r="E60" s="99" t="s">
         <v>13</v>
       </c>
@@ -27710,7 +27713,7 @@
       </c>
     </row>
     <row r="61" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D61" s="120"/>
+      <c r="D61" s="136"/>
       <c r="E61" s="99" t="s">
         <v>18</v>
       </c>
@@ -27768,7 +27771,7 @@
       </c>
     </row>
     <row r="62" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D62" s="121"/>
+      <c r="D62" s="137"/>
       <c r="E62" s="100"/>
       <c r="F62" s="100"/>
       <c r="G62" s="100"/>
@@ -27785,7 +27788,7 @@
       <c r="R62" s="100"/>
     </row>
     <row r="63" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D63" s="119">
+      <c r="D63" s="135">
         <f>DATE(selected_year, 3, 1)</f>
         <v>44621</v>
       </c>
@@ -27846,7 +27849,7 @@
       </c>
     </row>
     <row r="64" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D64" s="120"/>
+      <c r="D64" s="136"/>
       <c r="E64" s="99" t="s">
         <v>13</v>
       </c>
@@ -27904,7 +27907,7 @@
       </c>
     </row>
     <row r="65" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D65" s="120"/>
+      <c r="D65" s="136"/>
       <c r="E65" s="99" t="s">
         <v>18</v>
       </c>
@@ -27962,7 +27965,7 @@
       </c>
     </row>
     <row r="66" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D66" s="121"/>
+      <c r="D66" s="137"/>
       <c r="E66" s="100"/>
       <c r="F66" s="100"/>
       <c r="G66" s="100"/>
@@ -27979,7 +27982,7 @@
       <c r="R66" s="100"/>
     </row>
     <row r="67" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D67" s="119">
+      <c r="D67" s="135">
         <f>DATE(selected_year, 4, 1)</f>
         <v>44652</v>
       </c>
@@ -28040,7 +28043,7 @@
       </c>
     </row>
     <row r="68" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D68" s="120"/>
+      <c r="D68" s="136"/>
       <c r="E68" s="99" t="s">
         <v>13</v>
       </c>
@@ -28098,7 +28101,7 @@
       </c>
     </row>
     <row r="69" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D69" s="120"/>
+      <c r="D69" s="136"/>
       <c r="E69" s="99" t="s">
         <v>18</v>
       </c>
@@ -28156,7 +28159,7 @@
       </c>
     </row>
     <row r="70" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D70" s="121"/>
+      <c r="D70" s="137"/>
       <c r="E70" s="100"/>
       <c r="F70" s="100"/>
       <c r="G70" s="100"/>
@@ -28173,7 +28176,7 @@
       <c r="R70" s="100"/>
     </row>
     <row r="71" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D71" s="119">
+      <c r="D71" s="135">
         <f>DATE(selected_year, 5, 1)</f>
         <v>44682</v>
       </c>
@@ -28234,7 +28237,7 @@
       </c>
     </row>
     <row r="72" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D72" s="120"/>
+      <c r="D72" s="136"/>
       <c r="E72" s="99" t="s">
         <v>13</v>
       </c>
@@ -28292,7 +28295,7 @@
       </c>
     </row>
     <row r="73" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D73" s="120"/>
+      <c r="D73" s="136"/>
       <c r="E73" s="99" t="s">
         <v>18</v>
       </c>
@@ -28350,7 +28353,7 @@
       </c>
     </row>
     <row r="74" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D74" s="121"/>
+      <c r="D74" s="137"/>
       <c r="E74" s="100"/>
       <c r="F74" s="100"/>
       <c r="G74" s="100"/>
@@ -28367,7 +28370,7 @@
       <c r="R74" s="100"/>
     </row>
     <row r="75" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D75" s="119">
+      <c r="D75" s="135">
         <f>DATE(selected_year, 6, 1)</f>
         <v>44713</v>
       </c>
@@ -28428,7 +28431,7 @@
       </c>
     </row>
     <row r="76" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D76" s="120"/>
+      <c r="D76" s="136"/>
       <c r="E76" s="99" t="s">
         <v>13</v>
       </c>
@@ -28486,7 +28489,7 @@
       </c>
     </row>
     <row r="77" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D77" s="120"/>
+      <c r="D77" s="136"/>
       <c r="E77" s="99" t="s">
         <v>18</v>
       </c>
@@ -28544,7 +28547,7 @@
       </c>
     </row>
     <row r="78" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D78" s="121"/>
+      <c r="D78" s="137"/>
       <c r="E78" s="100"/>
       <c r="F78" s="100"/>
       <c r="G78" s="100"/>
@@ -28561,7 +28564,7 @@
       <c r="R78" s="100"/>
     </row>
     <row r="79" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D79" s="119">
+      <c r="D79" s="135">
         <f>DATE(selected_year, 7, 1)</f>
         <v>44743</v>
       </c>
@@ -28622,7 +28625,7 @@
       </c>
     </row>
     <row r="80" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D80" s="120"/>
+      <c r="D80" s="136"/>
       <c r="E80" s="99" t="s">
         <v>13</v>
       </c>
@@ -28680,7 +28683,7 @@
       </c>
     </row>
     <row r="81" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D81" s="120"/>
+      <c r="D81" s="136"/>
       <c r="E81" s="99" t="s">
         <v>18</v>
       </c>
@@ -28738,7 +28741,7 @@
       </c>
     </row>
     <row r="82" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D82" s="121"/>
+      <c r="D82" s="137"/>
       <c r="E82" s="100"/>
       <c r="F82" s="100"/>
       <c r="G82" s="100"/>
@@ -28755,7 +28758,7 @@
       <c r="R82" s="100"/>
     </row>
     <row r="83" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D83" s="119">
+      <c r="D83" s="135">
         <f>DATE(selected_year, 8, 1)</f>
         <v>44774</v>
       </c>
@@ -28816,7 +28819,7 @@
       </c>
     </row>
     <row r="84" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D84" s="120"/>
+      <c r="D84" s="136"/>
       <c r="E84" s="99" t="s">
         <v>13</v>
       </c>
@@ -28874,7 +28877,7 @@
       </c>
     </row>
     <row r="85" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D85" s="120"/>
+      <c r="D85" s="136"/>
       <c r="E85" s="99" t="s">
         <v>18</v>
       </c>
@@ -28932,7 +28935,7 @@
       </c>
     </row>
     <row r="86" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D86" s="121"/>
+      <c r="D86" s="137"/>
       <c r="E86" s="100"/>
       <c r="F86" s="100"/>
       <c r="G86" s="100"/>
@@ -28949,7 +28952,7 @@
       <c r="R86" s="100"/>
     </row>
     <row r="87" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D87" s="119">
+      <c r="D87" s="135">
         <f>DATE(selected_year, 9, 1)</f>
         <v>44805</v>
       </c>
@@ -29010,7 +29013,7 @@
       </c>
     </row>
     <row r="88" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D88" s="120"/>
+      <c r="D88" s="136"/>
       <c r="E88" s="99" t="s">
         <v>13</v>
       </c>
@@ -29068,7 +29071,7 @@
       </c>
     </row>
     <row r="89" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D89" s="120"/>
+      <c r="D89" s="136"/>
       <c r="E89" s="99" t="s">
         <v>18</v>
       </c>
@@ -29126,7 +29129,7 @@
       </c>
     </row>
     <row r="90" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D90" s="121"/>
+      <c r="D90" s="137"/>
       <c r="E90" s="100"/>
       <c r="F90" s="100"/>
       <c r="G90" s="100"/>
@@ -29143,7 +29146,7 @@
       <c r="R90" s="100"/>
     </row>
     <row r="91" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D91" s="119">
+      <c r="D91" s="135">
         <f>DATE(selected_year, 10, 1)</f>
         <v>44835</v>
       </c>
@@ -29204,7 +29207,7 @@
       </c>
     </row>
     <row r="92" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D92" s="120"/>
+      <c r="D92" s="136"/>
       <c r="E92" s="99" t="s">
         <v>13</v>
       </c>
@@ -29262,7 +29265,7 @@
       </c>
     </row>
     <row r="93" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D93" s="120"/>
+      <c r="D93" s="136"/>
       <c r="E93" s="99" t="s">
         <v>18</v>
       </c>
@@ -29320,7 +29323,7 @@
       </c>
     </row>
     <row r="94" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D94" s="121"/>
+      <c r="D94" s="137"/>
       <c r="E94" s="100"/>
       <c r="F94" s="100"/>
       <c r="G94" s="100"/>
@@ -29337,7 +29340,7 @@
       <c r="R94" s="100"/>
     </row>
     <row r="95" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D95" s="119">
+      <c r="D95" s="135">
         <f>DATE(selected_year, 11, 1)</f>
         <v>44866</v>
       </c>
@@ -29398,7 +29401,7 @@
       </c>
     </row>
     <row r="96" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D96" s="120"/>
+      <c r="D96" s="136"/>
       <c r="E96" s="99" t="s">
         <v>13</v>
       </c>
@@ -29456,7 +29459,7 @@
       </c>
     </row>
     <row r="97" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D97" s="120"/>
+      <c r="D97" s="136"/>
       <c r="E97" s="99" t="s">
         <v>18</v>
       </c>
@@ -29514,7 +29517,7 @@
       </c>
     </row>
     <row r="98" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D98" s="121"/>
+      <c r="D98" s="137"/>
       <c r="E98" s="100"/>
       <c r="F98" s="100"/>
       <c r="G98" s="100"/>
@@ -29531,7 +29534,7 @@
       <c r="R98" s="100"/>
     </row>
     <row r="99" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D99" s="119">
+      <c r="D99" s="135">
         <f>DATE(selected_year, 12, 1)</f>
         <v>44896</v>
       </c>
@@ -29592,7 +29595,7 @@
       </c>
     </row>
     <row r="100" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D100" s="120"/>
+      <c r="D100" s="136"/>
       <c r="E100" s="99" t="s">
         <v>13</v>
       </c>
@@ -29650,7 +29653,7 @@
       </c>
     </row>
     <row r="101" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D101" s="120"/>
+      <c r="D101" s="136"/>
       <c r="E101" s="99" t="s">
         <v>18</v>
       </c>
@@ -29708,7 +29711,7 @@
       </c>
     </row>
     <row r="102" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D102" s="121"/>
+      <c r="D102" s="137"/>
       <c r="E102" s="100"/>
       <c r="F102" s="100"/>
       <c r="G102" s="100"/>
@@ -29771,13 +29774,13 @@
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:5" s="126" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" s="126" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="42" t="s">
         <v>59</v>

</xml_diff>